<commit_message>
Ej Horas Operarios comenzado
</commit_message>
<xml_diff>
--- a/Dia2/Challenge_EjHoras/Personal.xlsx
+++ b/Dia2/Challenge_EjHoras/Personal.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desarrollo\DevPlace\Dia2\Challenge_EjHoras\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98619E4-375D-4587-BE86-FE6ADB7CD07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="18135" yWindow="4230" windowWidth="11025" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,37 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Pedro Perez</t>
+  </si>
+  <si>
+    <t>Juan Gopnzalez</t>
+  </si>
+  <si>
+    <t>Pablo Picapiedras</t>
+  </si>
+  <si>
+    <t>Marcelo Gomez</t>
+  </si>
+  <si>
+    <t>Alberto Paredes</t>
+  </si>
+  <si>
+    <t>Sebastian Romani</t>
+  </si>
+  <si>
+    <t>Mauricio Morales</t>
+  </si>
+  <si>
+    <t>Facundo Fredes</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +366,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>80.5</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>80.5</v>
+      </c>
+      <c r="D2">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>80.5</v>
+      </c>
+      <c r="D3">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>80.5</v>
+      </c>
+      <c r="D4">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>80.5</v>
+      </c>
+      <c r="D5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>80.5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>80.5</v>
+      </c>
+      <c r="D7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>80.5</v>
+      </c>
+      <c r="D8">
+        <v>3.5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>